<commit_message>
começo do minerador de dados
</commit_message>
<xml_diff>
--- a/delegacias.xlsx
+++ b/delegacias.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
   <si>
     <t xml:space="preserve">endereço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codRequest</t>
   </si>
   <si>
     <t xml:space="preserve">001 DP - Sé</t>
@@ -833,7 +836,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1029,16 +1032,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I105" activeCellId="0" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="88.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="88.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,949 +1052,1306 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1410</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1246</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1067</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1015</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>983</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>957</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>934</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>915</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1478</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1265</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1262</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1259</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1257</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1255</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1254</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1253</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1252</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1154</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1153</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1151</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1148</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1147</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1146</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1145</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1078</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1077</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1076</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1075</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1074</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1073</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1072</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>1071</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1070</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1069</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1027</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1026</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1025</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1024</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1023</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1022</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1021</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1020</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>1019</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1018</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>994</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>993</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>992</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>991</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>990</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>989</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>988</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>987</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>986</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>985</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>966</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>965</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>964</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>963</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>962</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>961</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>960</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>959</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>945</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>943</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>942</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>941</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>940</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>938</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>937</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>926</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>925</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>923</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>921</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>919</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>917</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>910</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>909</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>908</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>907</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>905</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>904</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>903</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>902</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>901</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>1270</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>1269</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>1268</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>1267</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>1251</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>1144</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>1068</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>1017</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>984</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>958</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>935</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>916</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>1476</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>773</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>772</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>771</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>764</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>758</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>1469</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>